<commit_message>
Optimizing sensor import code. Cleaned up some filenames.
</commit_message>
<xml_diff>
--- a/Data/LCR Physical Data.xlsx
+++ b/Data/LCR Physical Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\BIOLOGICAL\Flyco\LCR\Data &amp; Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\BIOLOGICAL\Flyco\LCR\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1741,11 +1741,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="196951784"/>
-        <c:axId val="197067224"/>
+        <c:axId val="454539552"/>
+        <c:axId val="454541120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="196951784"/>
+        <c:axId val="454539552"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1831,14 +1831,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197067224"/>
+        <c:crossAx val="454541120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
         <c:minorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="197067224"/>
+        <c:axId val="454541120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1924,7 +1924,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196951784"/>
+        <c:crossAx val="454539552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -2994,11 +2994,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="153057144"/>
-        <c:axId val="451386968"/>
+        <c:axId val="454540336"/>
+        <c:axId val="203683488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="153057144"/>
+        <c:axId val="454540336"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3084,14 +3084,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451386968"/>
+        <c:crossAx val="203683488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
         <c:minorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="451386968"/>
+        <c:axId val="203683488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3177,7 +3177,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153057144"/>
+        <c:crossAx val="454540336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -4748,6 +4748,134 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:v>2016-06</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'SpC Data'!$B$154:$B$165</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'SpC Data'!$C$154:$C$165</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4950</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4650</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4650</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4950</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4650</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4350</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -4756,11 +4884,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="197328688"/>
-        <c:axId val="197329080"/>
+        <c:axId val="203683880"/>
+        <c:axId val="203683096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="197328688"/>
+        <c:axId val="203683880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4873,12 +5001,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197329080"/>
+        <c:crossAx val="203683096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="197329080"/>
+        <c:axId val="203683096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4991,7 +5119,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197328688"/>
+        <c:crossAx val="203683880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11063,11 +11191,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G153"/>
+  <dimension ref="A1:G165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A101" sqref="A101:G142"/>
+      <selection pane="bottomLeft" activeCell="D166" sqref="D166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13562,6 +13690,174 @@
         <v>21</v>
       </c>
     </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="26">
+        <v>42545</v>
+      </c>
+      <c r="B154">
+        <v>10.4</v>
+      </c>
+      <c r="C154">
+        <v>4500</v>
+      </c>
+      <c r="D154">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="26">
+        <v>42545</v>
+      </c>
+      <c r="B155">
+        <v>11</v>
+      </c>
+      <c r="C155">
+        <v>4950</v>
+      </c>
+      <c r="D155">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="26">
+        <v>42545</v>
+      </c>
+      <c r="B156">
+        <v>12</v>
+      </c>
+      <c r="C156">
+        <v>4500</v>
+      </c>
+      <c r="D156">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="26">
+        <v>42545</v>
+      </c>
+      <c r="B157">
+        <v>13</v>
+      </c>
+      <c r="C157">
+        <v>4600</v>
+      </c>
+      <c r="D157">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="26">
+        <v>42545</v>
+      </c>
+      <c r="B158">
+        <v>14</v>
+      </c>
+      <c r="C158">
+        <v>4650</v>
+      </c>
+      <c r="D158">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="26">
+        <v>42545</v>
+      </c>
+      <c r="B159">
+        <v>15</v>
+      </c>
+      <c r="C159">
+        <v>4650</v>
+      </c>
+      <c r="D159">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="26">
+        <v>42545</v>
+      </c>
+      <c r="B160">
+        <v>16.2</v>
+      </c>
+      <c r="C160">
+        <v>4700</v>
+      </c>
+      <c r="D160">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="26">
+        <v>42545</v>
+      </c>
+      <c r="B161">
+        <v>17</v>
+      </c>
+      <c r="C161">
+        <v>4950</v>
+      </c>
+      <c r="D161">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="26">
+        <v>42545</v>
+      </c>
+      <c r="B162">
+        <v>18</v>
+      </c>
+      <c r="C162">
+        <v>4650</v>
+      </c>
+      <c r="D162">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="26">
+        <v>42545</v>
+      </c>
+      <c r="B163">
+        <v>19</v>
+      </c>
+      <c r="C163">
+        <v>4350</v>
+      </c>
+      <c r="D163">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="26">
+        <v>42545</v>
+      </c>
+      <c r="B164">
+        <v>20</v>
+      </c>
+      <c r="C164">
+        <v>4300</v>
+      </c>
+      <c r="D164">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="26">
+        <v>42545</v>
+      </c>
+      <c r="B165">
+        <v>20.75</v>
+      </c>
+      <c r="C165">
+        <v>4050</v>
+      </c>
+      <c r="D165">
+        <v>21.5</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A101:G142">
     <sortCondition ref="B101:B142"/>

</xml_diff>